<commit_message>
Correct inconsistent sizing behaviour
This just means setting some max-widths and min-widths around the
place
</commit_message>
<xml_diff>
--- a/TestCases/CreateStatSummarySheets/TalismanTestData.xlsx
+++ b/TestCases/CreateStatSummarySheets/TalismanTestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C03B350-C5D4-4407-BF7C-15F62C252C73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0ADCE6E-49A4-46E8-BF21-E3016CF66BEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="21600" windowHeight="11385" firstSheet="128" activeTab="134" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2715" yWindow="2985" windowWidth="21600" windowHeight="11385" firstSheet="132" activeTab="138" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sapphire" sheetId="1" r:id="rId1"/>
@@ -143,6 +143,10 @@
     <sheet name="STDEVPA (12)" sheetId="133" r:id="rId133"/>
     <sheet name="MIN (10)" sheetId="134" r:id="rId134"/>
     <sheet name="MAX (10)" sheetId="135" r:id="rId135"/>
+    <sheet name="AVERAGE (13)" sheetId="136" r:id="rId136"/>
+    <sheet name="STDEVPA (13)" sheetId="137" r:id="rId137"/>
+    <sheet name="MIN (11)" sheetId="138" r:id="rId138"/>
+    <sheet name="MAX (11)" sheetId="139" r:id="rId139"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -162,7 +166,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2815" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2895" uniqueCount="34">
   <si>
     <t>Email</t>
   </si>
@@ -6645,7 +6649,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F20D2A6-92AB-4A5A-B1D7-00DE4626EAA1}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
@@ -6784,6 +6788,598 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{3617000E-A3D8-48B5-B54A-45E03F6EBDC7}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet136.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75F70A15-DD22-4E1C-AE7A-7763891DF01E}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="6" max="6" width="53.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="e">
+        <f>AVERAGE(Sapphire:Sophie!$A$1)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="23" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="23"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="23"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F5" s="23"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F6" s="23"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="13"/>
+      <c r="F7" s="23"/>
+    </row>
+    <row r="8" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <f>AVERAGE(Sapphire:Sophie!$A$8)</f>
+        <v>4.8666666666666663</v>
+      </c>
+      <c r="B8" s="6">
+        <f>AVERAGE(Sapphire:Sophie!$B$8)</f>
+        <v>4.0666666666666664</v>
+      </c>
+      <c r="C8" s="8">
+        <f>AVERAGE(Sapphire:Sophie!$C$8)</f>
+        <v>4.8666666666666663</v>
+      </c>
+      <c r="D8" s="7">
+        <f>AVERAGE(Sapphire:Sophie!$D$8)</f>
+        <v>3.1333333333333333</v>
+      </c>
+      <c r="E8" s="14"/>
+      <c r="F8" s="23"/>
+    </row>
+    <row r="9" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D9" s="9"/>
+      <c r="F9" s="11"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="12"/>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="16">
+        <f>AVERAGE(Sapphire:Sophie!$B$11)</f>
+        <v>4.2333333333333334</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F2:F8"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{6E2810D8-6B57-4F7E-ABA4-5FE59A920EA2}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet137.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCAB1C66-A269-42F6-B89D-3E9AADD660EC}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="6" max="6" width="53.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2">
+        <f>STDEVPA(Sapphire:Sophie!$A$1)</f>
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="23" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="23"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="23"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F5" s="23"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F6" s="23"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="13"/>
+      <c r="F7" s="23"/>
+    </row>
+    <row r="8" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <f>STDEVPA(Sapphire:Sophie!$A$8)</f>
+        <v>0.33993463423951903</v>
+      </c>
+      <c r="B8" s="6">
+        <f>STDEVPA(Sapphire:Sophie!$B$8)</f>
+        <v>0.24944382578492932</v>
+      </c>
+      <c r="C8" s="8">
+        <f>STDEVPA(Sapphire:Sophie!$C$8)</f>
+        <v>0.33993463423951903</v>
+      </c>
+      <c r="D8" s="7">
+        <f>STDEVPA(Sapphire:Sophie!$D$8)</f>
+        <v>0.49888765156985887</v>
+      </c>
+      <c r="E8" s="14"/>
+      <c r="F8" s="23"/>
+    </row>
+    <row r="9" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D9" s="9"/>
+      <c r="F9" s="11"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="12"/>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="16">
+        <f>STDEVPA(Sapphire:Sophie!$B$11)</f>
+        <v>6.2360956446232331E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F2:F8"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{A0F0827F-73CF-4A3C-A215-22D13295F1ED}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet138.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0A43FB8-1086-47B1-AC1A-43016460D5B6}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="6" max="6" width="53.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2">
+        <f>MIN(Sapphire:Sophie!$A$1)</f>
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="23" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="23"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="23"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F5" s="23"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F6" s="23"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="13"/>
+      <c r="F7" s="23"/>
+    </row>
+    <row r="8" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <f>MIN(Sapphire:Sophie!$A$8)</f>
+        <v>4</v>
+      </c>
+      <c r="B8" s="6">
+        <f>MIN(Sapphire:Sophie!$B$8)</f>
+        <v>4</v>
+      </c>
+      <c r="C8" s="8">
+        <f>MIN(Sapphire:Sophie!$C$8)</f>
+        <v>4</v>
+      </c>
+      <c r="D8" s="7">
+        <f>MIN(Sapphire:Sophie!$D$8)</f>
+        <v>3</v>
+      </c>
+      <c r="E8" s="14"/>
+      <c r="F8" s="23"/>
+    </row>
+    <row r="9" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D9" s="9"/>
+      <c r="F9" s="11"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="12"/>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="16">
+        <f>MIN(Sapphire:Sophie!$B$11)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F2:F8"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{EF0D3195-8C5A-4B58-9F7D-1F282425D825}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet139.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABE41986-D968-49B1-B5FE-180A91A5E1CE}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="6" max="6" width="53.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2">
+        <f>MAX(Sapphire:Sophie!$A$1)</f>
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="23" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="23"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="23"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F5" s="23"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F6" s="23"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="13"/>
+      <c r="F7" s="23"/>
+    </row>
+    <row r="8" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <f>MAX(Sapphire:Sophie!$A$8)</f>
+        <v>5</v>
+      </c>
+      <c r="B8" s="6">
+        <f>MAX(Sapphire:Sophie!$B$8)</f>
+        <v>5</v>
+      </c>
+      <c r="C8" s="8">
+        <f>MAX(Sapphire:Sophie!$C$8)</f>
+        <v>5</v>
+      </c>
+      <c r="D8" s="7">
+        <f>MAX(Sapphire:Sophie!$D$8)</f>
+        <v>5</v>
+      </c>
+      <c r="E8" s="14"/>
+      <c r="F8" s="23"/>
+    </row>
+    <row r="9" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D9" s="9"/>
+      <c r="F9" s="11"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="12"/>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="16">
+        <f>MAX(Sapphire:Sophie!$B$11)</f>
+        <v>4.25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F2:F8"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{50906700-91EB-4B33-85FE-B1BC0DA7D8DA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Create 'Tabulate' project and test case
</commit_message>
<xml_diff>
--- a/TestCases/CreateStatSummarySheets/TalismanTestData.xlsx
+++ b/TestCases/CreateStatSummarySheets/TalismanTestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0ADCE6E-49A4-46E8-BF21-E3016CF66BEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB2335C5-02E6-4CB0-876A-C3E40008B53C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2715" yWindow="2985" windowWidth="21600" windowHeight="11385" firstSheet="132" activeTab="138" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1425" yWindow="1425" windowWidth="21600" windowHeight="11385" firstSheet="136" activeTab="142" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sapphire" sheetId="1" r:id="rId1"/>
@@ -147,6 +147,10 @@
     <sheet name="STDEVPA (13)" sheetId="137" r:id="rId137"/>
     <sheet name="MIN (11)" sheetId="138" r:id="rId138"/>
     <sheet name="MAX (11)" sheetId="139" r:id="rId139"/>
+    <sheet name="AVERAGE (14)" sheetId="140" r:id="rId140"/>
+    <sheet name="STDEVPA (14)" sheetId="141" r:id="rId141"/>
+    <sheet name="MIN (12)" sheetId="142" r:id="rId142"/>
+    <sheet name="MAX (12)" sheetId="143" r:id="rId143"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -166,7 +170,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2895" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2975" uniqueCount="34">
   <si>
     <t>Email</t>
   </si>
@@ -7241,7 +7245,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABE41986-D968-49B1-B5FE-180A91A5E1CE}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
@@ -7522,6 +7526,594 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{430FB083-FAC3-4F84-A5B0-99B581B3FE88}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet140.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64CDDD5A-37B4-4B55-B9A1-9C39CB7256FD}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="6" max="6" width="53.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="e">
+        <f>AVERAGE(Jeremy!$A$1)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="23" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="23"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="23"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F5" s="23"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F6" s="23"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="21"/>
+      <c r="F7" s="23"/>
+    </row>
+    <row r="8" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <f>AVERAGE(Jeremy!$A$8)</f>
+        <v>5</v>
+      </c>
+      <c r="B8" s="6">
+        <f>AVERAGE(Jeremy!$B$8)</f>
+        <v>4</v>
+      </c>
+      <c r="C8" s="22">
+        <f>AVERAGE(Jeremy!$C$8)</f>
+        <v>5</v>
+      </c>
+      <c r="D8" s="20">
+        <f>AVERAGE(Jeremy!$D$8)</f>
+        <v>3</v>
+      </c>
+      <c r="E8" s="19"/>
+      <c r="F8" s="23"/>
+    </row>
+    <row r="9" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F9" s="23"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="17"/>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="16">
+        <f>AVERAGE(Jeremy!$B$11)</f>
+        <v>4.25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F2:F9"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{C34B755E-112B-45D1-BEB3-D8763570F89E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet141.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F064137-6C43-4B94-BAA8-7463E558F50F}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="6" max="6" width="53.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2">
+        <f>STDEVPA(Jeremy!$A$1)</f>
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="23" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="23"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="23"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F5" s="23"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F6" s="23"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="21"/>
+      <c r="F7" s="23"/>
+    </row>
+    <row r="8" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <f>STDEVPA(Jeremy!$A$8)</f>
+        <v>0</v>
+      </c>
+      <c r="B8" s="6">
+        <f>STDEVPA(Jeremy!$B$8)</f>
+        <v>0</v>
+      </c>
+      <c r="C8" s="22">
+        <f>STDEVPA(Jeremy!$C$8)</f>
+        <v>0</v>
+      </c>
+      <c r="D8" s="20">
+        <f>STDEVPA(Jeremy!$D$8)</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="19"/>
+      <c r="F8" s="23"/>
+    </row>
+    <row r="9" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F9" s="23"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="17"/>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="16">
+        <f>STDEVPA(Jeremy!$B$11)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F2:F9"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{B3C3C463-4209-4580-ADE8-7F2CC3A9D249}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet142.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34196F56-5CB9-4574-8872-1FE0C16648FE}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="6" max="6" width="53.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2">
+        <f>MIN(Jeremy!$A$1)</f>
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="23" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="23"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="23"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F5" s="23"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F6" s="23"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="21"/>
+      <c r="F7" s="23"/>
+    </row>
+    <row r="8" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <f>MIN(Jeremy!$A$8)</f>
+        <v>5</v>
+      </c>
+      <c r="B8" s="6">
+        <f>MIN(Jeremy!$B$8)</f>
+        <v>4</v>
+      </c>
+      <c r="C8" s="22">
+        <f>MIN(Jeremy!$C$8)</f>
+        <v>5</v>
+      </c>
+      <c r="D8" s="20">
+        <f>MIN(Jeremy!$D$8)</f>
+        <v>3</v>
+      </c>
+      <c r="E8" s="19"/>
+      <c r="F8" s="23"/>
+    </row>
+    <row r="9" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F9" s="23"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="17"/>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="16">
+        <f>MIN(Jeremy!$B$11)</f>
+        <v>4.25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F2:F9"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{4AE64D2B-5FFD-4310-AB7A-3B4DD60DAE0C}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet143.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49B0F31B-47E1-432F-AA28-B4BC94546D5D}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="6" max="6" width="53.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2">
+        <f>MAX(Jeremy!$A$1)</f>
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="23" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="23"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="23"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F5" s="23"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F6" s="23"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="21"/>
+      <c r="F7" s="23"/>
+    </row>
+    <row r="8" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <f>MAX(Jeremy!$A$8)</f>
+        <v>5</v>
+      </c>
+      <c r="B8" s="6">
+        <f>MAX(Jeremy!$B$8)</f>
+        <v>4</v>
+      </c>
+      <c r="C8" s="22">
+        <f>MAX(Jeremy!$C$8)</f>
+        <v>5</v>
+      </c>
+      <c r="D8" s="20">
+        <f>MAX(Jeremy!$D$8)</f>
+        <v>3</v>
+      </c>
+      <c r="E8" s="19"/>
+      <c r="F8" s="23"/>
+    </row>
+    <row r="9" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F9" s="23"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="17"/>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="16">
+        <f>MAX(Jeremy!$B$11)</f>
+        <v>4.25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F2:F9"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{99E32C0C-2651-4104-B7B0-F7888200B4A5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>